<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@335cf1506496613d7fee64d0a3158d102be66a4a 🚀
</commit_message>
<xml_diff>
--- a/2022/raw.xlsx
+++ b/2022/raw.xlsx
@@ -2607,7 +2607,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2625,6 +2625,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -18192,8 +18195,8 @@
       <c r="Q298" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R298" s="4">
-        <v>87000.0</v>
+      <c r="R298" s="6">
+        <v>7250.0</v>
       </c>
       <c r="S298" s="4">
         <v>148000.0</v>
@@ -22681,7 +22684,7 @@
       <c r="R386" s="4">
         <v>2600.0</v>
       </c>
-      <c r="S386" s="6">
+      <c r="S386" s="7">
         <v>32500.0</v>
       </c>
       <c r="T386" s="1"/>
@@ -25405,7 +25408,7 @@
       <c r="Q439" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R439" s="7">
+      <c r="R439" s="8">
         <v>3300.0</v>
       </c>
       <c r="S439" s="4">
@@ -35995,7 +35998,7 @@
       <c r="Q645" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R645" s="8">
+      <c r="R645" s="9">
         <v>4460.0</v>
       </c>
       <c r="S645" s="4">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@00bd84bd6f9b39bf109953db6acb81569b63f424 🚀
</commit_message>
<xml_diff>
--- a/2022/raw.xlsx
+++ b/2022/raw.xlsx
@@ -2772,6 +2772,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="46.75"/>
+    <col customWidth="1" min="16" max="16" width="46.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">

</xml_diff>